<commit_message>
added DataExtractor modules and example excel output
</commit_message>
<xml_diff>
--- a/src/output_files/default/excel/MasterFile _ IPETRO PLANT_modified.xlsx
+++ b/src/output_files/default/excel/MasterFile _ IPETRO PLANT_modified.xlsx
@@ -19216,7 +19216,11 @@
       <c r="J8" s="40" t="n">
         <v>70</v>
       </c>
-      <c r="K8" s="41" t="n"/>
+      <c r="K8" s="41" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
       <c r="L8" s="41" t="n">
         <v>100</v>
       </c>
@@ -19274,7 +19278,11 @@
       <c r="J9" s="40" t="n">
         <v>70</v>
       </c>
-      <c r="K9" s="41" t="n"/>
+      <c r="K9" s="41" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
       <c r="L9" s="41" t="n">
         <v>100</v>
       </c>
@@ -19332,7 +19340,11 @@
       <c r="J10" s="40" t="n">
         <v>70</v>
       </c>
-      <c r="K10" s="41" t="n"/>
+      <c r="K10" s="41" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
       <c r="L10" s="41" t="n">
         <v>100</v>
       </c>
@@ -19386,19 +19398,43 @@
           <t>Liquid</t>
         </is>
       </c>
-      <c r="G11" s="40" t="n"/>
+      <c r="G11" s="40" t="inlineStr">
+        <is>
+          <t>CHILLED WATER</t>
+        </is>
+      </c>
       <c r="H11" s="95" t="inlineStr">
         <is>
           <t>Stainless Steel</t>
         </is>
       </c>
-      <c r="I11" s="40" t="n"/>
-      <c r="J11" s="40" t="n"/>
-      <c r="K11" s="41" t="n"/>
-      <c r="L11" s="41" t="n"/>
-      <c r="M11" s="96" t="n"/>
-      <c r="N11" s="41" t="n"/>
-      <c r="O11" s="96" t="n"/>
+      <c r="I11" s="40" t="inlineStr">
+        <is>
+          <t>SA-240</t>
+        </is>
+      </c>
+      <c r="J11" s="40" t="inlineStr">
+        <is>
+          <t>316L</t>
+        </is>
+      </c>
+      <c r="K11" s="41" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
+      <c r="L11" s="41" t="n">
+        <v>100</v>
+      </c>
+      <c r="M11" s="96" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="N11" s="41" t="n">
+        <v>100</v>
+      </c>
+      <c r="O11" s="96" t="n">
+        <v>1</v>
+      </c>
       <c r="P11" s="97" t="n"/>
       <c r="Q11" s="97" t="n"/>
       <c r="R11" s="97" t="n"/>
@@ -19428,7 +19464,7 @@
       </c>
       <c r="G12" s="40" t="inlineStr">
         <is>
-          <t>Water</t>
+          <t>CHILLED WATER</t>
         </is>
       </c>
       <c r="H12" s="95" t="inlineStr">
@@ -19436,15 +19472,33 @@
           <t>Stainless Steel</t>
         </is>
       </c>
-      <c r="I12" s="40" t="n"/>
-      <c r="J12" s="40" t="n"/>
-      <c r="K12" s="41" t="n"/>
+      <c r="I12" s="40" t="inlineStr">
+        <is>
+          <t>SA-240</t>
+        </is>
+      </c>
+      <c r="J12" s="40" t="inlineStr">
+        <is>
+          <t>316L</t>
+        </is>
+      </c>
+      <c r="K12" s="41" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
       <c r="L12" s="41" t="n">
-        <v>150</v>
-      </c>
-      <c r="M12" s="96" t="n"/>
-      <c r="N12" s="41" t="n"/>
-      <c r="O12" s="96" t="n"/>
+        <v>100</v>
+      </c>
+      <c r="M12" s="96" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="N12" s="41" t="n">
+        <v>100</v>
+      </c>
+      <c r="O12" s="96" t="n">
+        <v>1</v>
+      </c>
       <c r="P12" s="97" t="n"/>
       <c r="Q12" s="97" t="n"/>
       <c r="R12" s="97" t="n"/>
@@ -19472,19 +19526,43 @@
           <t>Liquid</t>
         </is>
       </c>
-      <c r="G13" s="40" t="n"/>
+      <c r="G13" s="40" t="inlineStr">
+        <is>
+          <t>CHILLED WATER</t>
+        </is>
+      </c>
       <c r="H13" s="95" t="inlineStr">
         <is>
           <t>Stainless Steel</t>
         </is>
       </c>
-      <c r="I13" s="40" t="n"/>
-      <c r="J13" s="40" t="n"/>
-      <c r="K13" s="41" t="n"/>
-      <c r="L13" s="41" t="n"/>
-      <c r="M13" s="96" t="n"/>
-      <c r="N13" s="41" t="n"/>
-      <c r="O13" s="96" t="n"/>
+      <c r="I13" s="40" t="inlineStr">
+        <is>
+          <t>SA-240</t>
+        </is>
+      </c>
+      <c r="J13" s="40" t="inlineStr">
+        <is>
+          <t>316L</t>
+        </is>
+      </c>
+      <c r="K13" s="41" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
+      <c r="L13" s="41" t="n">
+        <v>100</v>
+      </c>
+      <c r="M13" s="96" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="N13" s="41" t="n">
+        <v>100</v>
+      </c>
+      <c r="O13" s="96" t="n">
+        <v>1</v>
+      </c>
       <c r="P13" s="97" t="n"/>
       <c r="Q13" s="97" t="n"/>
       <c r="R13" s="97" t="n"/>
@@ -19660,19 +19738,43 @@
           <t>Liquid</t>
         </is>
       </c>
-      <c r="G17" s="40" t="n"/>
+      <c r="G17" s="40" t="inlineStr">
+        <is>
+          <t>Not found (no "FLUID NAME" field with "HOT WATER" value located)</t>
+        </is>
+      </c>
       <c r="H17" s="95" t="inlineStr">
         <is>
           <t>Stainless Steel</t>
         </is>
       </c>
-      <c r="I17" s="40" t="n"/>
-      <c r="J17" s="40" t="n"/>
-      <c r="K17" s="41" t="n"/>
-      <c r="L17" s="41" t="n"/>
-      <c r="M17" s="96" t="n"/>
-      <c r="N17" s="98" t="n"/>
-      <c r="O17" s="96" t="n"/>
+      <c r="I17" s="40" t="inlineStr">
+        <is>
+          <t>Not found (no "SHELL PLATE, ASTM A240 304L" entry located in Bill of Materials)</t>
+        </is>
+      </c>
+      <c r="J17" s="40" t="inlineStr">
+        <is>
+          <t>Not found</t>
+        </is>
+      </c>
+      <c r="K17" s="41" t="inlineStr">
+        <is>
+          <t>not found (no "insulation/personal protection" field with "hot insulation 100mm" located)</t>
+        </is>
+      </c>
+      <c r="L17" s="41" t="n">
+        <v>120</v>
+      </c>
+      <c r="M17" s="96" t="n">
+        <v>4</v>
+      </c>
+      <c r="N17" s="98" t="n">
+        <v>90</v>
+      </c>
+      <c r="O17" s="96" t="n">
+        <v>1</v>
+      </c>
       <c r="P17" s="97" t="n"/>
       <c r="Q17" s="97" t="n"/>
       <c r="R17" s="97" t="n"/>
@@ -19700,19 +19802,43 @@
           <t>Liquid</t>
         </is>
       </c>
-      <c r="G18" s="40" t="n"/>
+      <c r="G18" s="40" t="inlineStr">
+        <is>
+          <t>Not found (no "FLUID NAME" field with "HOT WATER" value located)</t>
+        </is>
+      </c>
       <c r="H18" s="95" t="inlineStr">
         <is>
           <t>Stainless Steel</t>
         </is>
       </c>
-      <c r="I18" s="40" t="n"/>
-      <c r="J18" s="40" t="n"/>
-      <c r="K18" s="41" t="n"/>
-      <c r="L18" s="41" t="n"/>
-      <c r="M18" s="96" t="n"/>
-      <c r="N18" s="98" t="n"/>
-      <c r="O18" s="96" t="n"/>
+      <c r="I18" s="40" t="inlineStr">
+        <is>
+          <t>Not found (no "SHELL PLATE, ASTM A240 304L" entry located in Bill of Materials)</t>
+        </is>
+      </c>
+      <c r="J18" s="40" t="inlineStr">
+        <is>
+          <t>Not found</t>
+        </is>
+      </c>
+      <c r="K18" s="41" t="inlineStr">
+        <is>
+          <t>not found (no "insulation/personal protection" field with "hot insulation 100mm" located)</t>
+        </is>
+      </c>
+      <c r="L18" s="41" t="n">
+        <v>120</v>
+      </c>
+      <c r="M18" s="96" t="n">
+        <v>4</v>
+      </c>
+      <c r="N18" s="98" t="n">
+        <v>90</v>
+      </c>
+      <c r="O18" s="96" t="n">
+        <v>1</v>
+      </c>
       <c r="P18" s="97" t="n"/>
       <c r="Q18" s="97" t="n"/>
       <c r="R18" s="97" t="n"/>
@@ -19754,19 +19880,43 @@
           <t>Liquid</t>
         </is>
       </c>
-      <c r="G19" s="40" t="n"/>
+      <c r="G19" s="40" t="inlineStr">
+        <is>
+          <t>WATER</t>
+        </is>
+      </c>
       <c r="H19" s="95" t="inlineStr">
         <is>
           <t>Stainless Steel</t>
         </is>
       </c>
-      <c r="I19" s="40" t="n"/>
-      <c r="J19" s="40" t="n"/>
-      <c r="K19" s="41" t="n"/>
-      <c r="L19" s="41" t="n"/>
-      <c r="M19" s="96" t="n"/>
-      <c r="N19" s="41" t="n"/>
-      <c r="O19" s="96" t="n"/>
+      <c r="I19" s="40" t="inlineStr">
+        <is>
+          <t>SA-240</t>
+        </is>
+      </c>
+      <c r="J19" s="40" t="inlineStr">
+        <is>
+          <t>316/316L</t>
+        </is>
+      </c>
+      <c r="K19" s="41" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="L19" s="41" t="n">
+        <v>150</v>
+      </c>
+      <c r="M19" s="96" t="n">
+        <v>4</v>
+      </c>
+      <c r="N19" s="41" t="n">
+        <v>45</v>
+      </c>
+      <c r="O19" s="96" t="n">
+        <v>0.52</v>
+      </c>
       <c r="P19" s="97" t="n"/>
       <c r="Q19" s="97" t="n"/>
       <c r="R19" s="97" t="n"/>
@@ -19794,19 +19944,45 @@
           <t>Liquid</t>
         </is>
       </c>
-      <c r="G20" s="40" t="n"/>
+      <c r="G20" s="40" t="inlineStr">
+        <is>
+          <t>AIR GAS/SULPHUR OXIDE</t>
+        </is>
+      </c>
       <c r="H20" s="95" t="inlineStr">
         <is>
           <t>Stainless Steel</t>
         </is>
       </c>
-      <c r="I20" s="40" t="n"/>
-      <c r="J20" s="40" t="n"/>
-      <c r="K20" s="41" t="n"/>
-      <c r="L20" s="41" t="n"/>
-      <c r="M20" s="96" t="n"/>
-      <c r="N20" s="41" t="n"/>
-      <c r="O20" s="96" t="n"/>
+      <c r="I20" s="40" t="inlineStr">
+        <is>
+          <t>SA-240</t>
+        </is>
+      </c>
+      <c r="J20" s="40" t="inlineStr">
+        <is>
+          <t>316/316L</t>
+        </is>
+      </c>
+      <c r="K20" s="41" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="L20" s="41" t="n">
+        <v>150</v>
+      </c>
+      <c r="M20" s="96" t="n">
+        <v>4</v>
+      </c>
+      <c r="N20" s="41" t="n">
+        <v>5.454015</v>
+      </c>
+      <c r="O20" s="96" t="inlineStr">
+        <is>
+          <t>0.5 / 2 / 3-4</t>
+        </is>
+      </c>
       <c r="P20" s="97" t="n"/>
       <c r="Q20" s="97" t="n"/>
       <c r="R20" s="97" t="n"/>
@@ -19834,19 +20010,43 @@
           <t>Gas</t>
         </is>
       </c>
-      <c r="G21" s="40" t="n"/>
+      <c r="G21" s="40" t="inlineStr">
+        <is>
+          <t>WATER</t>
+        </is>
+      </c>
       <c r="H21" s="95" t="inlineStr">
         <is>
           <t>Stainless Steel</t>
         </is>
       </c>
-      <c r="I21" s="40" t="n"/>
-      <c r="J21" s="40" t="n"/>
-      <c r="K21" s="41" t="n"/>
-      <c r="L21" s="41" t="n"/>
-      <c r="M21" s="96" t="n"/>
-      <c r="N21" s="41" t="n"/>
-      <c r="O21" s="96" t="n"/>
+      <c r="I21" s="40" t="inlineStr">
+        <is>
+          <t>SA-240</t>
+        </is>
+      </c>
+      <c r="J21" s="40" t="inlineStr">
+        <is>
+          <t>316/316L</t>
+        </is>
+      </c>
+      <c r="K21" s="41" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="L21" s="41" t="n">
+        <v>150</v>
+      </c>
+      <c r="M21" s="96" t="n">
+        <v>4</v>
+      </c>
+      <c r="N21" s="41" t="n">
+        <v>45</v>
+      </c>
+      <c r="O21" s="96" t="n">
+        <v>0.52</v>
+      </c>
       <c r="P21" s="97" t="n"/>
       <c r="Q21" s="97" t="n"/>
       <c r="R21" s="97" t="n"/>
@@ -19874,19 +20074,43 @@
           <t>Gas</t>
         </is>
       </c>
-      <c r="G22" s="40" t="n"/>
+      <c r="G22" s="40" t="inlineStr">
+        <is>
+          <t>WATER</t>
+        </is>
+      </c>
       <c r="H22" s="95" t="inlineStr">
         <is>
           <t>Stainless Steel</t>
         </is>
       </c>
-      <c r="I22" s="40" t="n"/>
-      <c r="J22" s="40" t="n"/>
-      <c r="K22" s="41" t="n"/>
-      <c r="L22" s="41" t="n"/>
-      <c r="M22" s="96" t="n"/>
-      <c r="N22" s="41" t="n"/>
-      <c r="O22" s="96" t="n"/>
+      <c r="I22" s="40" t="inlineStr">
+        <is>
+          <t>SA-240</t>
+        </is>
+      </c>
+      <c r="J22" s="40" t="inlineStr">
+        <is>
+          <t>316/316L</t>
+        </is>
+      </c>
+      <c r="K22" s="41" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="L22" s="41" t="n">
+        <v>150</v>
+      </c>
+      <c r="M22" s="96" t="n">
+        <v>4</v>
+      </c>
+      <c r="N22" s="41" t="n">
+        <v>45</v>
+      </c>
+      <c r="O22" s="96" t="n">
+        <v>0.52</v>
+      </c>
       <c r="P22" s="97" t="n"/>
       <c r="Q22" s="97" t="n"/>
       <c r="R22" s="97" t="n"/>
@@ -20220,15 +20444,31 @@
           <t>Liquid</t>
         </is>
       </c>
-      <c r="G28" s="40" t="n"/>
+      <c r="G28" s="40" t="inlineStr">
+        <is>
+          <t>ALKALINE WATER</t>
+        </is>
+      </c>
       <c r="H28" s="95" t="inlineStr">
         <is>
           <t>Stainless Steel</t>
         </is>
       </c>
-      <c r="I28" s="40" t="n"/>
-      <c r="J28" s="40" t="n"/>
-      <c r="K28" s="41" t="n"/>
+      <c r="I28" s="40" t="inlineStr">
+        <is>
+          <t>SA-403</t>
+        </is>
+      </c>
+      <c r="J28" s="40" t="inlineStr">
+        <is>
+          <t>WP316</t>
+        </is>
+      </c>
+      <c r="K28" s="41" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
       <c r="L28" s="41" t="n"/>
       <c r="M28" s="100" t="n"/>
       <c r="N28" s="41" t="n">
@@ -20264,15 +20504,31 @@
           <t>Liquid</t>
         </is>
       </c>
-      <c r="G29" s="40" t="n"/>
+      <c r="G29" s="40" t="inlineStr">
+        <is>
+          <t>CHILLED WATER</t>
+        </is>
+      </c>
       <c r="H29" s="95" t="inlineStr">
         <is>
           <t>Stainless Steel</t>
         </is>
       </c>
-      <c r="I29" s="40" t="n"/>
-      <c r="J29" s="40" t="n"/>
-      <c r="K29" s="41" t="n"/>
+      <c r="I29" s="40" t="inlineStr">
+        <is>
+          <t>SA-312</t>
+        </is>
+      </c>
+      <c r="J29" s="40" t="inlineStr">
+        <is>
+          <t>TP316</t>
+        </is>
+      </c>
+      <c r="K29" s="41" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
       <c r="L29" s="41" t="n"/>
       <c r="M29" s="100" t="n"/>
       <c r="N29" s="41" t="n">
@@ -20308,15 +20564,31 @@
           <t>Liquid</t>
         </is>
       </c>
-      <c r="G30" s="40" t="n"/>
+      <c r="G30" s="40" t="inlineStr">
+        <is>
+          <t>ALKALINE WATER</t>
+        </is>
+      </c>
       <c r="H30" s="95" t="inlineStr">
         <is>
           <t>Stainless Steel</t>
         </is>
       </c>
-      <c r="I30" s="40" t="n"/>
-      <c r="J30" s="40" t="n"/>
-      <c r="K30" s="41" t="n"/>
+      <c r="I30" s="40" t="inlineStr">
+        <is>
+          <t>SA-403</t>
+        </is>
+      </c>
+      <c r="J30" s="40" t="inlineStr">
+        <is>
+          <t>WP316</t>
+        </is>
+      </c>
+      <c r="K30" s="41" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
       <c r="L30" s="41" t="n"/>
       <c r="M30" s="100" t="n"/>
       <c r="N30" s="41" t="n">
@@ -20366,15 +20638,31 @@
           <t>Liquid</t>
         </is>
       </c>
-      <c r="G31" s="40" t="n"/>
+      <c r="G31" s="40" t="inlineStr">
+        <is>
+          <t>Chilled Water</t>
+        </is>
+      </c>
       <c r="H31" s="95" t="inlineStr">
         <is>
           <t>Stainless Steel</t>
         </is>
       </c>
-      <c r="I31" s="40" t="n"/>
-      <c r="J31" s="40" t="n"/>
-      <c r="K31" s="41" t="n"/>
+      <c r="I31" s="40" t="inlineStr">
+        <is>
+          <t>SA-403</t>
+        </is>
+      </c>
+      <c r="J31" s="40" t="inlineStr">
+        <is>
+          <t>316</t>
+        </is>
+      </c>
+      <c r="K31" s="41" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
       <c r="L31" s="41" t="n"/>
       <c r="M31" s="96" t="n"/>
       <c r="N31" s="41" t="n">
@@ -20410,15 +20698,31 @@
           <t>Liquid</t>
         </is>
       </c>
-      <c r="G32" s="40" t="n"/>
+      <c r="G32" s="40" t="inlineStr">
+        <is>
+          <t>REFLUX WATER</t>
+        </is>
+      </c>
       <c r="H32" s="95" t="inlineStr">
         <is>
           <t>Stainless Steel</t>
         </is>
       </c>
-      <c r="I32" s="40" t="n"/>
-      <c r="J32" s="40" t="n"/>
-      <c r="K32" s="41" t="n"/>
+      <c r="I32" s="40" t="inlineStr">
+        <is>
+          <t>SA-312</t>
+        </is>
+      </c>
+      <c r="J32" s="40" t="inlineStr">
+        <is>
+          <t>TP316</t>
+        </is>
+      </c>
+      <c r="K32" s="41" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
       <c r="L32" s="41" t="n"/>
       <c r="M32" s="96" t="n"/>
       <c r="N32" s="41" t="n">
@@ -20454,15 +20758,31 @@
           <t>Liquid</t>
         </is>
       </c>
-      <c r="G33" s="40" t="n"/>
+      <c r="G33" s="40" t="inlineStr">
+        <is>
+          <t>Chilled Water</t>
+        </is>
+      </c>
       <c r="H33" s="95" t="inlineStr">
         <is>
           <t>Stainless Steel</t>
         </is>
       </c>
-      <c r="I33" s="40" t="n"/>
-      <c r="J33" s="40" t="n"/>
-      <c r="K33" s="41" t="n"/>
+      <c r="I33" s="40" t="inlineStr">
+        <is>
+          <t>SA-403</t>
+        </is>
+      </c>
+      <c r="J33" s="40" t="inlineStr">
+        <is>
+          <t>316</t>
+        </is>
+      </c>
+      <c r="K33" s="41" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
       <c r="L33" s="41" t="n"/>
       <c r="M33" s="96" t="n"/>
       <c r="N33" s="41" t="n">
@@ -20512,15 +20832,31 @@
           <t>Liquid</t>
         </is>
       </c>
-      <c r="G34" s="40" t="n"/>
+      <c r="G34" s="40" t="inlineStr">
+        <is>
+          <t>CHILLED WATER</t>
+        </is>
+      </c>
       <c r="H34" s="95" t="inlineStr">
         <is>
           <t>Stainless Steel</t>
         </is>
       </c>
-      <c r="I34" s="40" t="n"/>
-      <c r="J34" s="40" t="n"/>
-      <c r="K34" s="41" t="n"/>
+      <c r="I34" s="40" t="inlineStr">
+        <is>
+          <t>SA-240</t>
+        </is>
+      </c>
+      <c r="J34" s="40" t="inlineStr">
+        <is>
+          <t>316/316L</t>
+        </is>
+      </c>
+      <c r="K34" s="41" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
       <c r="L34" s="41" t="n"/>
       <c r="M34" s="96" t="n"/>
       <c r="N34" s="41" t="n">
@@ -20556,15 +20892,31 @@
           <t>Liquid</t>
         </is>
       </c>
-      <c r="G35" s="40" t="n"/>
+      <c r="G35" s="40" t="inlineStr">
+        <is>
+          <t>REFLUX WATER</t>
+        </is>
+      </c>
       <c r="H35" s="95" t="inlineStr">
         <is>
           <t>Stainless Steel</t>
         </is>
       </c>
-      <c r="I35" s="40" t="n"/>
-      <c r="J35" s="40" t="n"/>
-      <c r="K35" s="41" t="n"/>
+      <c r="I35" s="40" t="inlineStr">
+        <is>
+          <t>SA-240</t>
+        </is>
+      </c>
+      <c r="J35" s="40" t="inlineStr">
+        <is>
+          <t>316/316L</t>
+        </is>
+      </c>
+      <c r="K35" s="41" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
       <c r="L35" s="41" t="n"/>
       <c r="M35" s="96" t="n"/>
       <c r="N35" s="41" t="n">
@@ -20600,15 +20952,31 @@
           <t>Liquid</t>
         </is>
       </c>
-      <c r="G36" s="40" t="n"/>
+      <c r="G36" s="40" t="inlineStr">
+        <is>
+          <t>CHILLED WATER</t>
+        </is>
+      </c>
       <c r="H36" s="95" t="inlineStr">
         <is>
           <t>Stainless Steel</t>
         </is>
       </c>
-      <c r="I36" s="40" t="n"/>
-      <c r="J36" s="40" t="n"/>
-      <c r="K36" s="41" t="n"/>
+      <c r="I36" s="40" t="inlineStr">
+        <is>
+          <t>SA-240</t>
+        </is>
+      </c>
+      <c r="J36" s="40" t="inlineStr">
+        <is>
+          <t>316/316L</t>
+        </is>
+      </c>
+      <c r="K36" s="41" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
       <c r="L36" s="41" t="n"/>
       <c r="M36" s="96" t="n"/>
       <c r="N36" s="41" t="n">

</xml_diff>